<commit_message>
updated sched and docs
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="15315" windowHeight="5955" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="15315" windowHeight="5955"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -15,14 +15,13 @@
     <sheet name="Sprint 5" sheetId="6" r:id="rId6"/>
     <sheet name="Sprint 6" sheetId="7" r:id="rId7"/>
     <sheet name="Sprint 7" sheetId="8" r:id="rId8"/>
-    <sheet name="Sprint 8" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="36">
   <si>
     <t>Product Backlog</t>
   </si>
@@ -34,9 +33,6 @@
   </si>
   <si>
     <t>3. Pause game</t>
-  </si>
-  <si>
-    <t>8. Change the color of the ball and stage</t>
   </si>
   <si>
     <t>7. Next stage</t>
@@ -121,9 +117,6 @@
     <t>Sprint 7: Next Stage</t>
   </si>
   <si>
-    <t>Sprint 8: Change the color of the ball and stage</t>
-  </si>
-  <si>
     <t>Actual</t>
   </si>
   <si>
@@ -134,9 +127,6 @@
   </si>
   <si>
     <t>Learning Curve</t>
-  </si>
-  <si>
-    <t>Designing and coding UI</t>
   </si>
   <si>
     <t xml:space="preserve">       Hours (Individual)</t>
@@ -158,9 +148,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
-    <numFmt numFmtId="165" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -207,14 +196,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -422,24 +408,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="74625792"/>
-        <c:axId val="74627328"/>
+        <c:axId val="58054144"/>
+        <c:axId val="58055680"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="74625792"/>
+        <c:axId val="58054144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="[$-409]mmmm\ d\,\ yyyy;@" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74627328"/>
+        <c:crossAx val="58055680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="74627328"/>
+        <c:axId val="58055680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -447,7 +433,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74625792"/>
+        <c:crossAx val="58054144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -458,9 +444,23 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -493,10 +493,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sprint 2'!$A$17:$A$24</c:f>
+              <c:f>'Sprint 2'!$A$17:$A$33</c:f>
               <c:numCache>
                 <c:formatCode>[$-409]mmmm\ d\,\ yyyy;@</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>42025</c:v>
                 </c:pt>
@@ -520,16 +520,43 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>42032</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>42033</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>42034</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>42035</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>42036</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42037</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>42038</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>42039</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>42040</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>42041</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 2'!$B$17:$B$24</c:f>
+              <c:f>'Sprint 2'!$B$17:$B$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>43</c:v>
                 </c:pt>
@@ -550,6 +577,36 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -574,10 +631,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sprint 2'!$A$17:$A$24</c:f>
+              <c:f>'Sprint 2'!$A$17:$A$33</c:f>
               <c:numCache>
                 <c:formatCode>[$-409]mmmm\ d\,\ yyyy;@</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>42025</c:v>
                 </c:pt>
@@ -601,16 +658,43 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>42032</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>42033</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>42034</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>42035</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>42036</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42037</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>42038</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>42039</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>42040</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>42041</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 2'!$C$17:$C$24</c:f>
+              <c:f>'Sprint 2'!$C$17:$C$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>44</c:v>
                 </c:pt>
@@ -640,24 +724,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="74652288"/>
-        <c:axId val="74674560"/>
+        <c:axId val="58600064"/>
+        <c:axId val="58618240"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="74652288"/>
+        <c:axId val="58600064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="[$-409]mmmm\ d\,\ yyyy;@" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74674560"/>
+        <c:crossAx val="58618240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="74674560"/>
+        <c:axId val="58618240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -665,7 +749,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74652288"/>
+        <c:crossAx val="58600064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -678,7 +762,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -697,7 +781,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sprint 3'!$B$15</c:f>
+              <c:f>'Sprint 3'!$B$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -711,40 +795,64 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sprint 3'!$A$16:$A$22</c:f>
+              <c:f>'Sprint 3'!$A$18:$A$26</c:f>
               <c:numCache>
                 <c:formatCode>[$-409]mmmm\ d\,\ yyyy;@</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>42033</c:v>
+                  <c:v>42042</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42034</c:v>
+                  <c:v>42043</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42035</c:v>
+                  <c:v>42044</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42036</c:v>
+                  <c:v>42045</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42037</c:v>
+                  <c:v>42046</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>42038</c:v>
+                  <c:v>42047</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>42039</c:v>
+                  <c:v>42048</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>42049</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>42050</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 3'!$B$16:$B$22</c:f>
+              <c:f>'Sprint 3'!$B$18:$B$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -754,7 +862,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sprint 3'!$C$15</c:f>
+              <c:f>'Sprint 3'!$C$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -768,59 +876,71 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sprint 3'!$A$16:$A$22</c:f>
+              <c:f>'Sprint 3'!$A$18:$A$26</c:f>
               <c:numCache>
                 <c:formatCode>[$-409]mmmm\ d\,\ yyyy;@</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>42033</c:v>
+                  <c:v>42042</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42034</c:v>
+                  <c:v>42043</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42035</c:v>
+                  <c:v>42044</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42036</c:v>
+                  <c:v>42045</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42037</c:v>
+                  <c:v>42046</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>42038</c:v>
+                  <c:v>42047</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>42039</c:v>
+                  <c:v>42048</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>42049</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>42050</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 3'!$C$16:$C$22</c:f>
+              <c:f>'Sprint 3'!$C$18:$C$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>42</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>38</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>36</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>28</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -828,24 +948,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="74998528"/>
-        <c:axId val="75000064"/>
+        <c:axId val="58680448"/>
+        <c:axId val="58681984"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="74998528"/>
+        <c:axId val="58680448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="[$-409]mmmm\ d\,\ yyyy;@" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75000064"/>
+        <c:crossAx val="58681984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="75000064"/>
+        <c:axId val="58681984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -853,7 +973,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74998528"/>
+        <c:crossAx val="58680448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -866,7 +986,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -899,40 +1019,34 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sprint 4'!$A$16:$A$22</c:f>
+              <c:f>'Sprint 4'!$A$16:$A$20</c:f>
               <c:numCache>
                 <c:formatCode>[$-409]mmmm\ d\,\ yyyy;@</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>42040</c:v>
+                  <c:v>42051</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42041</c:v>
+                  <c:v>42052</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42042</c:v>
+                  <c:v>42053</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42043</c:v>
+                  <c:v>42054</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42044</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>42045</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>42046</c:v>
+                  <c:v>42055</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 4'!$B$16:$B$22</c:f>
+              <c:f>'Sprint 4'!$B$16:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="5"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -956,59 +1070,47 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sprint 4'!$A$16:$A$22</c:f>
+              <c:f>'Sprint 4'!$A$16:$A$20</c:f>
               <c:numCache>
                 <c:formatCode>[$-409]mmmm\ d\,\ yyyy;@</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>42040</c:v>
+                  <c:v>42051</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42041</c:v>
+                  <c:v>42052</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42042</c:v>
+                  <c:v>42053</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42043</c:v>
+                  <c:v>42054</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42044</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>42045</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>42046</c:v>
+                  <c:v>42055</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 4'!$C$16:$C$22</c:f>
+              <c:f>'Sprint 4'!$C$16:$C$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>34</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>32</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1016,24 +1118,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="76163712"/>
-        <c:axId val="76173696"/>
+        <c:axId val="59780096"/>
+        <c:axId val="59785984"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="76163712"/>
+        <c:axId val="59780096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="[$-409]mmmm\ d\,\ yyyy;@" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76173696"/>
+        <c:crossAx val="59785984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="76173696"/>
+        <c:axId val="59785984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1041,7 +1143,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76163712"/>
+        <c:crossAx val="59780096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1054,7 +1156,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1087,43 +1189,37 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sprint 5'!$A$17:$A$24</c:f>
+              <c:f>'Sprint 5'!$A$17:$A$22</c:f>
               <c:numCache>
                 <c:formatCode>[$-409]mmmm\ d\,\ yyyy;@</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>42047</c:v>
+                  <c:v>42056</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42048</c:v>
+                  <c:v>42057</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42049</c:v>
+                  <c:v>42058</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42050</c:v>
+                  <c:v>42059</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42051</c:v>
+                  <c:v>42060</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>42052</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>42053</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>42054</c:v>
+                  <c:v>42061</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 5'!$B$17:$B$24</c:f>
+              <c:f>'Sprint 5'!$B$17:$B$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="6"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1147,65 +1243,53 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sprint 5'!$A$17:$A$24</c:f>
+              <c:f>'Sprint 5'!$A$17:$A$22</c:f>
               <c:numCache>
                 <c:formatCode>[$-409]mmmm\ d\,\ yyyy;@</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>42047</c:v>
+                  <c:v>42056</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42048</c:v>
+                  <c:v>42057</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42049</c:v>
+                  <c:v>42058</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42050</c:v>
+                  <c:v>42059</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42051</c:v>
+                  <c:v>42060</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>42052</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>42053</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>42054</c:v>
+                  <c:v>42061</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 5'!$C$17:$C$24</c:f>
+              <c:f>'Sprint 5'!$C$17:$C$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>40</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>36</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>32</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1213,24 +1297,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="76108160"/>
-        <c:axId val="76109696"/>
+        <c:axId val="59859712"/>
+        <c:axId val="59861248"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="76108160"/>
+        <c:axId val="59859712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="[$-409]mmmm\ d\,\ yyyy;@" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76109696"/>
+        <c:crossAx val="59861248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="76109696"/>
+        <c:axId val="59861248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1238,7 +1322,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76108160"/>
+        <c:crossAx val="59859712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1251,7 +1335,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1284,37 +1368,34 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sprint 6'!$A$15:$A$20</c:f>
+              <c:f>'Sprint 6'!$A$15:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>[$-409]mmmm\ d\,\ yyyy;@</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>42055</c:v>
+                  <c:v>42062</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42056</c:v>
+                  <c:v>42063</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42057</c:v>
+                  <c:v>42064</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42058</c:v>
+                  <c:v>42065</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42059</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>42060</c:v>
+                  <c:v>42066</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 6'!$B$15:$B$20</c:f>
+              <c:f>'Sprint 6'!$B$15:$B$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1338,53 +1419,47 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sprint 6'!$A$15:$A$20</c:f>
+              <c:f>'Sprint 6'!$A$15:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>[$-409]mmmm\ d\,\ yyyy;@</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>42055</c:v>
+                  <c:v>42062</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42056</c:v>
+                  <c:v>42063</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42057</c:v>
+                  <c:v>42064</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42058</c:v>
+                  <c:v>42065</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42059</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>42060</c:v>
+                  <c:v>42066</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 6'!$C$15:$C$20</c:f>
+              <c:f>'Sprint 6'!$C$15:$C$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>38</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1392,24 +1467,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="76142848"/>
-        <c:axId val="76148736"/>
+        <c:axId val="59890304"/>
+        <c:axId val="59896192"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="76142848"/>
+        <c:axId val="59890304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="[$-409]mmmm\ d\,\ yyyy;@" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76148736"/>
+        <c:crossAx val="59896192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="76148736"/>
+        <c:axId val="59896192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1417,7 +1492,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76142848"/>
+        <c:crossAx val="59890304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1430,7 +1505,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1463,37 +1538,34 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sprint 7'!$A$15:$A$20</c:f>
+              <c:f>'Sprint 7'!$A$15:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>[$-409]mmmm\ d\,\ yyyy;@</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>42061</c:v>
+                  <c:v>42067</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42062</c:v>
+                  <c:v>42068</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42063</c:v>
+                  <c:v>42069</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42064</c:v>
+                  <c:v>42070</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42065</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>42066</c:v>
+                  <c:v>42071</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 7'!$B$15:$B$20</c:f>
+              <c:f>'Sprint 7'!$B$15:$B$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1517,53 +1589,47 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sprint 7'!$A$15:$A$20</c:f>
+              <c:f>'Sprint 7'!$A$15:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>[$-409]mmmm\ d\,\ yyyy;@</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>42061</c:v>
+                  <c:v>42067</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42062</c:v>
+                  <c:v>42068</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42063</c:v>
+                  <c:v>42069</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42064</c:v>
+                  <c:v>42070</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42065</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>42066</c:v>
+                  <c:v>42071</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 7'!$C$15:$C$20</c:f>
+              <c:f>'Sprint 7'!$C$15:$C$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>34</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>28</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1571,24 +1637,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="76358016"/>
-        <c:axId val="76359552"/>
+        <c:axId val="60109568"/>
+        <c:axId val="60111104"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="76358016"/>
+        <c:axId val="60109568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="[$-409]mmmm\ d\,\ yyyy;@" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76359552"/>
+        <c:crossAx val="60111104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="76359552"/>
+        <c:axId val="60111104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1596,7 +1662,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76358016"/>
+        <c:crossAx val="60109568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1609,168 +1675,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:chart>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Sprint 8'!$B$12</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Actual</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Sprint 8'!$A$13:$A$16</c:f>
-              <c:numCache>
-                <c:formatCode>[$-409]mmmm\ d\,\ yyyy;@</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>42067</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>42068</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>42069</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>42070</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sprint 8'!$B$13:$B$16</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Sprint 8'!$C$12</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Ideal</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Sprint 8'!$A$13:$A$16</c:f>
-              <c:numCache>
-                <c:formatCode>[$-409]mmmm\ d\,\ yyyy;@</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>42067</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>42068</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>42069</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>42070</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sprint 8'!$C$13:$C$16</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:marker val="1"/>
-        <c:axId val="76400896"/>
-        <c:axId val="76410880"/>
-      </c:lineChart>
-      <c:dateAx>
-        <c:axId val="76400896"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="[$-409]mmmm\ d\,\ yyyy;@" sourceLinked="1"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76410880"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblOffset val="100"/>
-      </c:dateAx>
-      <c:valAx>
-        <c:axId val="76410880"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76400896"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1815,20 +1720,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="5" name="Chart 4"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1851,19 +1756,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1886,19 +1791,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1921,19 +1826,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1956,19 +1861,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
+      <xdr:colOff>123825</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
+      <xdr:colOff>85725</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="4" name="Chart 3"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1991,54 +1896,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>628650</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>752475</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2343,8 +2213,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2361,15 +2231,15 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="B3" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="6" t="s">
+      <c r="B3" s="6" t="s">
         <v>31</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2399,15 +2269,15 @@
         <v>3</v>
       </c>
       <c r="B6">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="C6">
-        <v>44</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>20</v>
@@ -2418,72 +2288,61 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C8">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C9">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C10">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B11">
-        <v>13</v>
+        <v>149</v>
       </c>
       <c r="C11">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>165</v>
-      </c>
-      <c r="C12">
-        <v>330</v>
+        <v>298</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -2496,8 +2355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2510,29 +2369,29 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="3">
+        <v>42016</v>
+      </c>
+      <c r="B5" t="s">
         <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="4">
-        <v>42016</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -2542,11 +2401,11 @@
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>42017</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -2556,11 +2415,11 @@
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <v>42018</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -2570,11 +2429,11 @@
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="4">
+      <c r="A8" s="3">
         <v>42019</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -2584,11 +2443,11 @@
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="4">
+      <c r="A9" s="3">
         <v>42020</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -2598,11 +2457,11 @@
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="4">
+      <c r="A10" s="3">
         <v>42021</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C10">
         <v>4</v>
@@ -2612,11 +2471,11 @@
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="4">
+      <c r="A11" s="3">
         <v>42022</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11">
         <v>6</v>
@@ -2626,11 +2485,11 @@
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="4">
+      <c r="A12" s="3">
         <v>42023</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12">
         <v>4</v>
@@ -2640,11 +2499,11 @@
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="4">
+      <c r="A13" s="3">
         <v>42024</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13">
         <v>4</v>
@@ -2655,8 +2514,8 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2"/>
-      <c r="B14" s="5" t="s">
-        <v>10</v>
+      <c r="B14" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="C14">
         <v>27</v>
@@ -2667,17 +2526,17 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="4">
+      <c r="A18" s="3">
         <v>42016</v>
       </c>
       <c r="B18">
@@ -2688,7 +2547,7 @@
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="4">
+      <c r="A19" s="3">
         <v>42017</v>
       </c>
       <c r="B19">
@@ -2699,7 +2558,7 @@
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="4">
+      <c r="A20" s="3">
         <v>42018</v>
       </c>
       <c r="B20">
@@ -2710,7 +2569,7 @@
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="4">
+      <c r="A21" s="3">
         <v>42019</v>
       </c>
       <c r="B21">
@@ -2721,7 +2580,7 @@
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="4">
+      <c r="A22" s="3">
         <v>42020</v>
       </c>
       <c r="B22">
@@ -2732,7 +2591,7 @@
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="4">
+      <c r="A23" s="3">
         <v>42021</v>
       </c>
       <c r="B23">
@@ -2743,7 +2602,7 @@
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="4">
+      <c r="A24" s="3">
         <v>42022</v>
       </c>
       <c r="B24">
@@ -2754,7 +2613,7 @@
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="4">
+      <c r="A25" s="3">
         <v>42023</v>
       </c>
       <c r="B25">
@@ -2765,7 +2624,7 @@
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="4">
+      <c r="A26" s="3">
         <v>42024</v>
       </c>
       <c r="B26">
@@ -2784,10 +2643,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2800,29 +2659,29 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="4">
+      <c r="A5" s="3">
         <v>42025</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -2832,11 +2691,11 @@
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>42026</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -2846,11 +2705,11 @@
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <v>42027</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -2860,11 +2719,11 @@
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="4">
+      <c r="A8" s="3">
         <v>42028</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C8">
         <v>4</v>
@@ -2874,11 +2733,11 @@
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="4">
+      <c r="A9" s="3">
         <v>42029</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9">
         <v>5</v>
@@ -2888,11 +2747,11 @@
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="4">
+      <c r="A10" s="3">
         <v>42030</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10">
         <v>5</v>
@@ -2902,11 +2761,11 @@
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="4">
+      <c r="A11" s="3">
         <v>42031</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11">
         <v>3</v>
@@ -2916,11 +2775,11 @@
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="4">
+      <c r="A12" s="3">
         <v>42032</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C12">
         <v>3</v>
@@ -2931,8 +2790,8 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2"/>
-      <c r="B13" s="5" t="s">
-        <v>10</v>
+      <c r="B13" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="C13">
         <v>23</v>
@@ -2946,17 +2805,17 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="4">
+      <c r="A17" s="3">
         <v>42025</v>
       </c>
       <c r="B17">
@@ -2967,7 +2826,7 @@
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="4">
+      <c r="A18" s="3">
         <v>42026</v>
       </c>
       <c r="B18">
@@ -2978,7 +2837,7 @@
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="4">
+      <c r="A19" s="3">
         <v>42027</v>
       </c>
       <c r="B19">
@@ -2989,7 +2848,7 @@
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="4">
+      <c r="A20" s="3">
         <v>42028</v>
       </c>
       <c r="B20">
@@ -3000,7 +2859,7 @@
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="4">
+      <c r="A21" s="3">
         <v>42029</v>
       </c>
       <c r="B21">
@@ -3011,7 +2870,7 @@
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="4">
+      <c r="A22" s="3">
         <v>42030</v>
       </c>
       <c r="B22">
@@ -3022,7 +2881,7 @@
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="4">
+      <c r="A23" s="3">
         <v>42031</v>
       </c>
       <c r="B23">
@@ -3033,25 +2892,101 @@
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="4">
+      <c r="A24" s="3">
         <v>42032</v>
+      </c>
+      <c r="B24">
+        <v>18</v>
       </c>
       <c r="C24">
         <v>0</v>
       </c>
     </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="3">
+        <v>42033</v>
+      </c>
+      <c r="B25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="3">
+        <v>42034</v>
+      </c>
+      <c r="B26">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="3">
+        <v>42035</v>
+      </c>
+      <c r="B27">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="3">
+        <v>42036</v>
+      </c>
+      <c r="B28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="3">
+        <v>42037</v>
+      </c>
+      <c r="B29">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="3">
+        <v>42038</v>
+      </c>
+      <c r="B30">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="3">
+        <v>42039</v>
+      </c>
+      <c r="B31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="3">
+        <v>42040</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="3">
+        <v>42041</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3064,29 +2999,29 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="4">
-        <v>42033</v>
+      <c r="A5" s="3">
+        <v>42042</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -3096,11 +3031,11 @@
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="4">
-        <v>42034</v>
+      <c r="A6" s="3">
+        <v>42043</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -3110,11 +3045,11 @@
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="4">
-        <v>42035</v>
+      <c r="A7" s="3">
+        <v>42044</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -3124,11 +3059,11 @@
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="4">
-        <v>42036</v>
+      <c r="A8" s="3">
+        <v>42045</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C8">
         <v>4</v>
@@ -3138,11 +3073,11 @@
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="4">
-        <v>42037</v>
+      <c r="A9" s="3">
+        <v>42046</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9">
         <v>6</v>
@@ -3152,11 +3087,11 @@
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="4">
-        <v>42038</v>
+      <c r="A10" s="3">
+        <v>42047</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C10">
         <v>4</v>
@@ -3166,11 +3101,11 @@
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="4">
-        <v>42039</v>
+      <c r="A11" s="3">
+        <v>42048</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C11">
         <v>4</v>
@@ -3180,90 +3115,149 @@
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="2"/>
-      <c r="B12" s="5" t="s">
-        <v>10</v>
+      <c r="A12" s="3">
+        <v>42049</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
       </c>
       <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="3">
+        <v>42050</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="B14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14">
+        <v>30</v>
+      </c>
+      <c r="D14">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="3">
+        <v>42042</v>
+      </c>
+      <c r="B18">
+        <v>56</v>
+      </c>
+      <c r="C18">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="3">
+        <v>42043</v>
+      </c>
+      <c r="B19">
+        <v>53</v>
+      </c>
+      <c r="C19">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="3">
+        <v>42044</v>
+      </c>
+      <c r="B20">
+        <v>50</v>
+      </c>
+      <c r="C20">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="3">
+        <v>42045</v>
+      </c>
+      <c r="B21">
+        <v>43</v>
+      </c>
+      <c r="C21">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="3">
+        <v>42046</v>
+      </c>
+      <c r="B22">
+        <v>31</v>
+      </c>
+      <c r="C22">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="3">
+        <v>42047</v>
+      </c>
+      <c r="B23">
         <v>22</v>
       </c>
-      <c r="D12">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="2"/>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="4">
-        <v>42033</v>
-      </c>
-      <c r="C16">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="4">
-        <v>42034</v>
-      </c>
-      <c r="C17">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="4">
-        <v>42035</v>
-      </c>
-      <c r="C18">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="4">
-        <v>42036</v>
-      </c>
-      <c r="C19">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="4">
-        <v>42037</v>
-      </c>
-      <c r="C20">
+      <c r="C23">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="3">
+        <v>42048</v>
+      </c>
+      <c r="C24">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="4">
-        <v>42038</v>
-      </c>
-      <c r="C21">
+    <row r="25" spans="1:3">
+      <c r="A25" s="3">
+        <v>42049</v>
+      </c>
+      <c r="C25">
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="4">
-        <v>42039</v>
-      </c>
-      <c r="C22">
+    <row r="26" spans="1:3">
+      <c r="A26" s="3">
+        <v>42050</v>
+      </c>
+      <c r="C26">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3271,8 +3265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3285,29 +3279,29 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="4">
-        <v>42040</v>
+      <c r="A5" s="3">
+        <v>42051</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -3317,39 +3311,39 @@
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="4">
-        <v>42041</v>
+      <c r="A6" s="3">
+        <v>42052</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D6">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="4">
-        <v>42042</v>
+      <c r="A7" s="3">
+        <v>42053</v>
       </c>
       <c r="B7" t="s">
         <v>17</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="4">
-        <v>42043</v>
+      <c r="A8" s="3">
+        <v>42054</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="C8">
         <v>4</v>
@@ -3359,11 +3353,11 @@
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="4">
-        <v>42044</v>
+      <c r="A9" s="3">
+        <v>42055</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C9">
         <v>6</v>
@@ -3373,114 +3367,82 @@
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="4">
-        <v>42045</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
+      <c r="A10" s="3"/>
+      <c r="B10" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="D10">
-        <v>6</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="4">
-        <v>42046</v>
-      </c>
-      <c r="B11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11">
-        <v>3</v>
-      </c>
-      <c r="D11">
-        <v>6</v>
-      </c>
+      <c r="A11" s="3"/>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2"/>
-      <c r="B12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12">
-        <v>20</v>
-      </c>
-      <c r="D12">
-        <v>40</v>
-      </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2"/>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="4">
-        <v>42040</v>
+      <c r="A16" s="3">
+        <v>42051</v>
       </c>
       <c r="C16">
         <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="4">
-        <v>42041</v>
+      <c r="A17" s="3">
+        <v>42052</v>
       </c>
       <c r="C17">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="4">
-        <v>42042</v>
+      <c r="A18" s="3">
+        <v>42053</v>
       </c>
       <c r="C18">
-        <v>32</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="4">
-        <v>42043</v>
+      <c r="A19" s="3">
+        <v>42054</v>
       </c>
       <c r="C19">
-        <v>24</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="4">
-        <v>42044</v>
+      <c r="A20" s="3">
+        <v>42055</v>
       </c>
       <c r="C20">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="4">
-        <v>42045</v>
-      </c>
-      <c r="C21">
-        <v>6</v>
-      </c>
+      <c r="A21" s="3"/>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="4">
-        <v>42046</v>
-      </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
+      <c r="A22" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3492,8 +3454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3506,29 +3468,29 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="4">
-        <v>42047</v>
+      <c r="A5" s="3">
+        <v>42056</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -3538,11 +3500,11 @@
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="4">
-        <v>42048</v>
+      <c r="A6" s="3">
+        <v>42057</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -3552,8 +3514,8 @@
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="4">
-        <v>42049</v>
+      <c r="A7" s="3">
+        <v>42058</v>
       </c>
       <c r="B7" t="s">
         <v>17</v>
@@ -3566,11 +3528,11 @@
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="4">
-        <v>42050</v>
+      <c r="A8" s="3">
+        <v>42059</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="C8">
         <v>4</v>
@@ -3580,8 +3542,8 @@
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="4">
-        <v>42051</v>
+      <c r="A9" s="3">
+        <v>42060</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
@@ -3594,11 +3556,11 @@
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="4">
-        <v>42052</v>
+      <c r="A10" s="3">
+        <v>42061</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C10">
         <v>3</v>
@@ -3608,118 +3570,84 @@
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="4">
-        <v>42053</v>
-      </c>
-      <c r="B11" t="s">
-        <v>19</v>
+      <c r="A11" s="3"/>
+      <c r="B11" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="D11">
-        <v>4</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="4">
-        <v>42054</v>
-      </c>
-      <c r="B12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12">
-        <v>3</v>
-      </c>
-      <c r="D12">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="B13" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13">
-        <v>21</v>
-      </c>
-      <c r="D13">
-        <v>42</v>
-      </c>
+      <c r="A12" s="3"/>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="3">
+        <v>42056</v>
+      </c>
+      <c r="C17">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="4">
-        <v>42047</v>
-      </c>
-      <c r="C17">
-        <v>40</v>
-      </c>
-    </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="4">
-        <v>42048</v>
+      <c r="A18" s="3">
+        <v>42057</v>
       </c>
       <c r="C18">
-        <v>36</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="4">
-        <v>42049</v>
+      <c r="A19" s="3">
+        <v>42058</v>
       </c>
       <c r="C19">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="4">
-        <v>42050</v>
+      <c r="A20" s="3">
+        <v>42059</v>
       </c>
       <c r="C20">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="4">
-        <v>42051</v>
+      <c r="A21" s="3">
+        <v>42060</v>
       </c>
       <c r="C21">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="4">
-        <v>42052</v>
+      <c r="A22" s="3">
+        <v>42061</v>
       </c>
       <c r="C22">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="4">
-        <v>42053</v>
-      </c>
-      <c r="C23">
-        <v>6</v>
-      </c>
+      <c r="A23" s="3"/>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="4">
-        <v>42054</v>
-      </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
+      <c r="A24" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3731,8 +3659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3745,29 +3673,29 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="4">
-        <v>42055</v>
+      <c r="A5" s="3">
+        <v>42062</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -3777,11 +3705,11 @@
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="4">
-        <v>42056</v>
+      <c r="A6" s="3">
+        <v>42063</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -3791,11 +3719,11 @@
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="4">
-        <v>42057</v>
+      <c r="A7" s="3">
+        <v>42064</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7">
         <v>5</v>
@@ -3805,8 +3733,8 @@
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="4">
-        <v>42058</v>
+      <c r="A8" s="3">
+        <v>42065</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
@@ -3819,11 +3747,11 @@
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="4">
-        <v>42059</v>
+      <c r="A9" s="3">
+        <v>42066</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C9">
         <v>3</v>
@@ -3833,92 +3761,76 @@
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="4">
-        <v>42060</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
+      <c r="A10" s="3"/>
+      <c r="B10" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="D10">
-        <v>6</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2"/>
-      <c r="B11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11">
-        <v>20</v>
-      </c>
-      <c r="D11">
-        <v>40</v>
-      </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2"/>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="4">
-        <v>42055</v>
+      <c r="A15" s="3">
+        <v>42062</v>
       </c>
       <c r="C15">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="4">
-        <v>42056</v>
+      <c r="A16" s="3">
+        <v>42063</v>
       </c>
       <c r="C16">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="4">
-        <v>42057</v>
+      <c r="A17" s="3">
+        <v>42064</v>
       </c>
       <c r="C17">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="4">
-        <v>42058</v>
+      <c r="A18" s="3">
+        <v>42065</v>
       </c>
       <c r="C18">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="4">
-        <v>42059</v>
+      <c r="A19" s="3">
+        <v>42066</v>
       </c>
       <c r="C19">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="4">
-        <v>42060</v>
-      </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
+      <c r="A20" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3930,8 +3842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3944,29 +3856,29 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="4">
-        <v>42061</v>
+      <c r="A5" s="3">
+        <v>42067</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -3976,11 +3888,11 @@
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="4">
-        <v>42062</v>
+      <c r="A6" s="3">
+        <v>42068</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -3990,11 +3902,11 @@
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="4">
-        <v>42063</v>
+      <c r="A7" s="3">
+        <v>42069</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7">
         <v>4</v>
@@ -4004,8 +3916,8 @@
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="4">
-        <v>42064</v>
+      <c r="A8" s="3">
+        <v>42070</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
@@ -4018,11 +3930,11 @@
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="4">
-        <v>42065</v>
+      <c r="A9" s="3">
+        <v>42071</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C9">
         <v>3</v>
@@ -4032,246 +3944,73 @@
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="4">
-        <v>42066</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
+      <c r="A10" s="3"/>
+      <c r="B10" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="D10">
-        <v>6</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2"/>
-      <c r="B11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11">
-        <v>19</v>
-      </c>
-      <c r="D11">
-        <v>38</v>
-      </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="4">
-        <v>42061</v>
+      <c r="A15" s="3">
+        <v>42067</v>
       </c>
       <c r="C15">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="4">
-        <v>42062</v>
+      <c r="A16" s="3">
+        <v>42068</v>
       </c>
       <c r="C16">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="4">
-        <v>42063</v>
+      <c r="A17" s="3">
+        <v>42069</v>
       </c>
       <c r="C17">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="4">
-        <v>42064</v>
+      <c r="A18" s="3">
+        <v>42070</v>
       </c>
       <c r="C18">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="4">
-        <v>42065</v>
+      <c r="A19" s="3">
+        <v>42071</v>
       </c>
       <c r="C19">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="4">
-        <v>42066</v>
-      </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="42" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" customWidth="1"/>
-    <col min="3" max="4" width="17.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="4">
-        <v>42067</v>
-      </c>
-      <c r="B5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-      <c r="D5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="4">
-        <v>42068</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6">
-        <v>4</v>
-      </c>
-      <c r="D6">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="4">
-        <v>42069</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="4">
-        <v>42070</v>
-      </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8">
-        <v>3</v>
-      </c>
-      <c r="D8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="4"/>
-      <c r="B9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9">
-        <v>13</v>
-      </c>
-      <c r="D9">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="3"/>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="2"/>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="4">
-        <v>42067</v>
-      </c>
-      <c r="C13">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="4">
-        <v>42068</v>
-      </c>
-      <c r="C14">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="4">
-        <v>42069</v>
-      </c>
-      <c r="C15">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="4">
-        <v>42070</v>
-      </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
+      <c r="A20" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
sprint 3 and 4 merged
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -4,24 +4,23 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="15315" windowHeight="5955" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="15315" windowHeight="5955" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
     <sheet name="Sprint 1" sheetId="2" r:id="rId2"/>
     <sheet name="Sprint 2" sheetId="3" r:id="rId3"/>
     <sheet name="Sprint 3" sheetId="4" r:id="rId4"/>
-    <sheet name="Sprint 4" sheetId="5" r:id="rId5"/>
-    <sheet name="Sprint 5" sheetId="6" r:id="rId6"/>
-    <sheet name="Sprint 6" sheetId="7" r:id="rId7"/>
-    <sheet name="Sprint 7" sheetId="8" r:id="rId8"/>
+    <sheet name="Sprint 4" sheetId="6" r:id="rId5"/>
+    <sheet name="Sprint 5" sheetId="7" r:id="rId6"/>
+    <sheet name="Sprint 6" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="37">
   <si>
     <t>Product Backlog</t>
   </si>
@@ -30,21 +29,6 @@
   </si>
   <si>
     <t>1. Play game</t>
-  </si>
-  <si>
-    <t>3. Pause game</t>
-  </si>
-  <si>
-    <t>7. Next stage</t>
-  </si>
-  <si>
-    <t>6. Post time online</t>
-  </si>
-  <si>
-    <t>4. Resume game</t>
-  </si>
-  <si>
-    <t>5. Restart game</t>
   </si>
   <si>
     <t>Hours (Individual)</t>
@@ -102,21 +86,6 @@
     <t>Code Debugging</t>
   </si>
   <si>
-    <t>Sprint 3: Pause Game</t>
-  </si>
-  <si>
-    <t>Sprint 4: Resume Game</t>
-  </si>
-  <si>
-    <t>Sprint 5: Restart Game</t>
-  </si>
-  <si>
-    <t>Sprint 6: Post Time  Online</t>
-  </si>
-  <si>
-    <t>Sprint 7: Next Stage</t>
-  </si>
-  <si>
     <t>Actual</t>
   </si>
   <si>
@@ -142,6 +111,39 @@
   </si>
   <si>
     <t>CSc 193</t>
+  </si>
+  <si>
+    <t>Sprint 3: Pause and Resume Game</t>
+  </si>
+  <si>
+    <t>Sprint 4: Restart Game</t>
+  </si>
+  <si>
+    <t>Sprint 5: Post Time  Online</t>
+  </si>
+  <si>
+    <t>Sprint 6: Next Stage</t>
+  </si>
+  <si>
+    <t>Designing and coding the UI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Designing and coding the UI </t>
+  </si>
+  <si>
+    <t>3. Pause and Resume game</t>
+  </si>
+  <si>
+    <t>4. Restart game</t>
+  </si>
+  <si>
+    <t>5. Post time online</t>
+  </si>
+  <si>
+    <t>6. Next stage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date </t>
   </si>
 </sst>
 </file>
@@ -408,24 +410,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="48568576"/>
-        <c:axId val="48599040"/>
+        <c:axId val="57202176"/>
+        <c:axId val="57203712"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="48568576"/>
+        <c:axId val="57202176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="[$-409]mmmm\ d\,\ yyyy;@" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48599040"/>
+        <c:crossAx val="57203712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="48599040"/>
+        <c:axId val="57203712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -433,13 +435,14 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48568576"/>
+        <c:crossAx val="57202176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -459,7 +462,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -723,24 +726,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="48622976"/>
-        <c:axId val="48624768"/>
+        <c:axId val="58600064"/>
+        <c:axId val="58618240"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="48622976"/>
+        <c:axId val="58600064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="[$-409]mmmm\ d\,\ yyyy;@" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48624768"/>
+        <c:crossAx val="58618240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="48624768"/>
+        <c:axId val="58618240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -748,19 +751,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48622976"/>
+        <c:crossAx val="58600064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -779,7 +783,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sprint 3'!$B$17</c:f>
+              <c:f>'Sprint 3'!$B$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -793,63 +797,114 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sprint 3'!$A$18:$A$26</c:f>
+              <c:f>'Sprint 3'!$A$29:$A$47</c:f>
               <c:numCache>
                 <c:formatCode>[$-409]mmmm\ d\,\ yyyy;@</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>42042</c:v>
+                  <c:v>42044</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42043</c:v>
+                  <c:v>42045</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42044</c:v>
+                  <c:v>42046</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42045</c:v>
+                  <c:v>42047</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42046</c:v>
+                  <c:v>42048</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>42047</c:v>
+                  <c:v>42049</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>42048</c:v>
+                  <c:v>42050</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>42049</c:v>
+                  <c:v>42051</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>42050</c:v>
+                  <c:v>42052</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>42053</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>42054</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>42055</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42056</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>42057</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>42058</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>42059</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>42060</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 3'!$B$18:$B$26</c:f>
+              <c:f>'Sprint 3'!$B$29:$B$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>57</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>52</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>50</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="7">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>43</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>22</c:v>
+                <c:pt idx="9">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -860,7 +915,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sprint 3'!$C$17</c:f>
+              <c:f>'Sprint 3'!$C$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -874,71 +929,119 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sprint 3'!$A$18:$A$26</c:f>
+              <c:f>'Sprint 3'!$A$29:$A$47</c:f>
               <c:numCache>
                 <c:formatCode>[$-409]mmmm\ d\,\ yyyy;@</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>42042</c:v>
+                  <c:v>42044</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42043</c:v>
+                  <c:v>42045</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42044</c:v>
+                  <c:v>42046</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42045</c:v>
+                  <c:v>42047</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42046</c:v>
+                  <c:v>42048</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>42047</c:v>
+                  <c:v>42049</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>42048</c:v>
+                  <c:v>42050</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>42049</c:v>
+                  <c:v>42051</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>42050</c:v>
+                  <c:v>42052</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>42053</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>42054</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>42055</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42056</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>42057</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>42058</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>42059</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>42060</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 3'!$C$18:$C$26</c:f>
+              <c:f>'Sprint 3'!$C$29:$C$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>58</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>54</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>52</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="7">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>44</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="9">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>32</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="11">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="14">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -946,24 +1049,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="50251648"/>
-        <c:axId val="50253184"/>
+        <c:axId val="56958976"/>
+        <c:axId val="56962432"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="50251648"/>
+        <c:axId val="56958976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="[$-409]mmmm\ d\,\ yyyy;@" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50253184"/>
+        <c:crossAx val="56962432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="50253184"/>
+        <c:axId val="56962432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -971,7 +1074,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50251648"/>
+        <c:crossAx val="56958976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -984,7 +1087,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1003,7 +1106,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sprint 4'!$B$15</c:f>
+              <c:f>'Sprint 4'!$B$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1017,34 +1120,31 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sprint 4'!$A$16:$A$20</c:f>
+              <c:f>'Sprint 4'!$A$13:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>[$-409]mmmm\ d\,\ yyyy;@</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>42051</c:v>
+                  <c:v>42061</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42052</c:v>
+                  <c:v>42062</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42053</c:v>
+                  <c:v>42063</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42054</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>42055</c:v>
+                  <c:v>42064</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 4'!$B$16:$B$20</c:f>
+              <c:f>'Sprint 4'!$B$13:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="4"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1054,7 +1154,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sprint 4'!$C$15</c:f>
+              <c:f>'Sprint 4'!$C$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1068,47 +1168,41 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sprint 4'!$A$16:$A$20</c:f>
+              <c:f>'Sprint 4'!$A$13:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>[$-409]mmmm\ d\,\ yyyy;@</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>42051</c:v>
+                  <c:v>42061</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42052</c:v>
+                  <c:v>42062</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42053</c:v>
+                  <c:v>42063</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42054</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>42055</c:v>
+                  <c:v>42064</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 4'!$C$16:$C$20</c:f>
+              <c:f>'Sprint 4'!$C$13:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>38</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1116,24 +1210,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="50434048"/>
-        <c:axId val="50435584"/>
+        <c:axId val="67472768"/>
+        <c:axId val="69878912"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="50434048"/>
+        <c:axId val="67472768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="[$-409]mmmm\ d\,\ yyyy;@" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50435584"/>
+        <c:crossAx val="69878912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="50435584"/>
+        <c:axId val="69878912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1141,19 +1235,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50434048"/>
+        <c:crossAx val="67472768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1172,7 +1267,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sprint 5'!$B$16</c:f>
+              <c:f>'Sprint 5'!$B$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1186,37 +1281,31 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sprint 5'!$A$17:$A$22</c:f>
+              <c:f>'Sprint 5'!$A$13:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>[$-409]mmmm\ d\,\ yyyy;@</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>42056</c:v>
+                  <c:v>42065</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42057</c:v>
+                  <c:v>42066</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42058</c:v>
+                  <c:v>42067</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42059</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>42060</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>42061</c:v>
+                  <c:v>42068</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 5'!$B$17:$B$22</c:f>
+              <c:f>'Sprint 5'!$B$13:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="4"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1226,7 +1315,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sprint 5'!$C$16</c:f>
+              <c:f>'Sprint 5'!$C$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1240,53 +1329,41 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sprint 5'!$A$17:$A$22</c:f>
+              <c:f>'Sprint 5'!$A$13:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>[$-409]mmmm\ d\,\ yyyy;@</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>42056</c:v>
+                  <c:v>42065</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42057</c:v>
+                  <c:v>42066</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42058</c:v>
+                  <c:v>42067</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42059</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>42060</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>42061</c:v>
+                  <c:v>42068</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 5'!$C$17:$C$22</c:f>
+              <c:f>'Sprint 5'!$C$13:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>30</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>26</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1294,24 +1371,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="50570752"/>
-        <c:axId val="50572288"/>
+        <c:axId val="70064768"/>
+        <c:axId val="70096768"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="50570752"/>
+        <c:axId val="70064768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="[$-409]mmmm\ d\,\ yyyy;@" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50572288"/>
+        <c:crossAx val="70096768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="50572288"/>
+        <c:axId val="70096768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1319,19 +1396,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50570752"/>
+        <c:crossAx val="70064768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1350,7 +1428,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sprint 6'!$B$14</c:f>
+              <c:f>'Sprint 6'!$B$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1364,34 +1442,31 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sprint 6'!$A$15:$A$19</c:f>
+              <c:f>'Sprint 6'!$A$13:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>[$-409]mmmm\ d\,\ yyyy;@</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>42062</c:v>
+                  <c:v>42069</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42063</c:v>
+                  <c:v>42070</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42064</c:v>
+                  <c:v>42071</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42065</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>42066</c:v>
+                  <c:v>42072</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 6'!$B$15:$B$19</c:f>
+              <c:f>'Sprint 6'!$B$13:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="4"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1401,7 +1476,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sprint 6'!$C$14</c:f>
+              <c:f>'Sprint 6'!$C$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1415,47 +1490,41 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sprint 6'!$A$15:$A$19</c:f>
+              <c:f>'Sprint 6'!$A$13:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>[$-409]mmmm\ d\,\ yyyy;@</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>42062</c:v>
+                  <c:v>42069</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42063</c:v>
+                  <c:v>42070</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42064</c:v>
+                  <c:v>42071</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42065</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>42066</c:v>
+                  <c:v>42072</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 6'!$C$15:$C$19</c:f>
+              <c:f>'Sprint 6'!$C$13:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>26</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1463,24 +1532,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="50593152"/>
-        <c:axId val="51119232"/>
+        <c:axId val="57635968"/>
+        <c:axId val="57637504"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="50593152"/>
+        <c:axId val="57635968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="[$-409]mmmm\ d\,\ yyyy;@" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51119232"/>
+        <c:crossAx val="57637504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="51119232"/>
+        <c:axId val="57637504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1488,188 +1557,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50593152"/>
+        <c:crossAx val="57635968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:chart>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Sprint 7'!$B$14</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Actual</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Sprint 7'!$A$15:$A$19</c:f>
-              <c:numCache>
-                <c:formatCode>[$-409]mmmm\ d\,\ yyyy;@</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>42067</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>42068</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>42069</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>42070</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>42071</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sprint 7'!$B$15:$B$19</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Sprint 7'!$C$14</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Ideal</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Sprint 7'!$A$15:$A$19</c:f>
-              <c:numCache>
-                <c:formatCode>[$-409]mmmm\ d\,\ yyyy;@</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>42067</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>42068</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>42069</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>42070</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>42071</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sprint 7'!$C$15:$C$19</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:marker val="1"/>
-        <c:axId val="48784896"/>
-        <c:axId val="48786432"/>
-      </c:lineChart>
-      <c:dateAx>
-        <c:axId val="48784896"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="[$-409]mmmm\ d\,\ yyyy;@" sourceLinked="1"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48786432"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblOffset val="100"/>
-      </c:dateAx>
-      <c:valAx>
-        <c:axId val="48786432"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48784896"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1749,20 +1650,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>133351</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>171451</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="5" name="Chart 4"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1785,19 +1686,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="5" name="Chart 4"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1820,15 +1721,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1855,54 +1756,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="4" name="Chart 3"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2207,8 +2073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2225,15 +2091,15 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="B3" s="6" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2260,83 +2126,72 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="B6">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="C6">
-        <v>60</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="B7">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C7">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="B8">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C8">
-        <v>32</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="B9">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C9">
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B10">
-        <v>16</v>
+        <v>151</v>
       </c>
       <c r="C10">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>149</v>
-      </c>
-      <c r="C11">
-        <v>298</v>
+        <v>302</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -2349,8 +2204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2363,21 +2218,21 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2385,7 +2240,7 @@
         <v>42016</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -2399,7 +2254,7 @@
         <v>42017</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -2413,7 +2268,7 @@
         <v>42018</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -2427,7 +2282,7 @@
         <v>42019</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -2441,7 +2296,7 @@
         <v>42020</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -2455,7 +2310,7 @@
         <v>42021</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C10">
         <v>4</v>
@@ -2469,7 +2324,7 @@
         <v>42022</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C11">
         <v>6</v>
@@ -2483,7 +2338,7 @@
         <v>42023</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C12">
         <v>4</v>
@@ -2497,7 +2352,7 @@
         <v>42024</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C13">
         <v>4</v>
@@ -2509,7 +2364,7 @@
     <row r="14" spans="1:4">
       <c r="A14" s="2"/>
       <c r="B14" s="4" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C14">
         <v>27</v>
@@ -2520,13 +2375,13 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -2639,7 +2494,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
@@ -2653,21 +2508,21 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2675,7 +2530,7 @@
         <v>42025</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -2689,7 +2544,7 @@
         <v>42026</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -2703,7 +2558,7 @@
         <v>42027</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -2717,7 +2572,7 @@
         <v>42028</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C8">
         <v>4</v>
@@ -2731,7 +2586,7 @@
         <v>42029</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C9">
         <v>5</v>
@@ -2745,7 +2600,7 @@
         <v>42030</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C10">
         <v>5</v>
@@ -2759,7 +2614,7 @@
         <v>42031</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C11">
         <v>3</v>
@@ -2773,7 +2628,7 @@
         <v>42032</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C12">
         <v>3</v>
@@ -2785,7 +2640,7 @@
     <row r="13" spans="1:4">
       <c r="A13" s="2"/>
       <c r="B13" s="4" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C13">
         <v>23</v>
@@ -2799,13 +2654,13 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -2977,15 +2832,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="1" max="1" width="31.5703125" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" customWidth="1"/>
     <col min="3" max="3" width="22.140625" customWidth="1"/>
     <col min="4" max="4" width="18.28515625" customWidth="1"/>
@@ -2993,21 +2848,21 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -3015,7 +2870,7 @@
         <v>42042</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -3029,13 +2884,13 @@
         <v>42043</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
         <v>2</v>
-      </c>
-      <c r="D6">
-        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -3043,7 +2898,7 @@
         <v>42044</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -3057,13 +2912,13 @@
         <v>42045</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
         <v>4</v>
-      </c>
-      <c r="D8">
-        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -3071,13 +2926,13 @@
         <v>42046</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C9">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D9">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -3085,13 +2940,13 @@
         <v>42047</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
         <v>4</v>
-      </c>
-      <c r="D10">
-        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -3099,13 +2954,13 @@
         <v>42048</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
         <v>4</v>
-      </c>
-      <c r="D11">
-        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -3113,13 +2968,13 @@
         <v>42049</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
         <v>4</v>
-      </c>
-      <c r="D12">
-        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -3127,124 +2982,381 @@
         <v>42050</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
         <v>4</v>
       </c>
-      <c r="D13">
-        <v>8</v>
-      </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="B14" s="4" t="s">
-        <v>9</v>
+      <c r="A14" s="3">
+        <v>42051</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
       </c>
       <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="3">
+        <v>42052</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="3">
+        <v>42053</v>
+      </c>
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="3">
+        <v>42054</v>
+      </c>
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="3">
+        <v>42055</v>
+      </c>
+      <c r="B18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="3">
+        <v>42056</v>
+      </c>
+      <c r="B19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="D19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="3">
+        <v>42057</v>
+      </c>
+      <c r="B20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="3">
+        <v>42058</v>
+      </c>
+      <c r="B21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="3">
+        <v>42059</v>
+      </c>
+      <c r="B22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="3">
+        <v>42060</v>
+      </c>
+      <c r="B23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="3"/>
+      <c r="B24" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24">
+        <v>41</v>
+      </c>
+      <c r="D24">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="3"/>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="3">
+        <v>42042</v>
+      </c>
+      <c r="B27">
+        <v>79</v>
+      </c>
+      <c r="C27">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="3">
+        <v>42043</v>
+      </c>
+      <c r="B28">
+        <v>77</v>
+      </c>
+      <c r="C28">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="3">
+        <v>42044</v>
+      </c>
+      <c r="B29">
+        <v>75</v>
+      </c>
+      <c r="C29">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="3">
+        <v>42045</v>
+      </c>
+      <c r="B30">
+        <v>70</v>
+      </c>
+      <c r="C30">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="3">
+        <v>42046</v>
+      </c>
+      <c r="B31">
+        <v>66</v>
+      </c>
+      <c r="C31">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="3">
+        <v>42047</v>
+      </c>
+      <c r="B32">
+        <v>62</v>
+      </c>
+      <c r="C32">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="3">
+        <v>42048</v>
+      </c>
+      <c r="B33">
+        <v>58</v>
+      </c>
+      <c r="C33">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="3">
+        <v>42049</v>
+      </c>
+      <c r="B34">
+        <v>55</v>
+      </c>
+      <c r="C34">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="3">
+        <v>42050</v>
+      </c>
+      <c r="B35">
+        <v>50</v>
+      </c>
+      <c r="C35">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="3">
+        <v>42051</v>
+      </c>
+      <c r="B36">
+        <v>46</v>
+      </c>
+      <c r="C36">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="3">
+        <v>42052</v>
+      </c>
+      <c r="B37">
+        <v>43</v>
+      </c>
+      <c r="C37">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="3">
+        <v>42053</v>
+      </c>
+      <c r="B38">
+        <v>36</v>
+      </c>
+      <c r="C38">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="3">
+        <v>42054</v>
+      </c>
+      <c r="B39">
         <v>30</v>
       </c>
-      <c r="D14">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="3">
-        <v>42042</v>
-      </c>
-      <c r="B18">
-        <v>57</v>
-      </c>
-      <c r="C18">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="3">
-        <v>42043</v>
-      </c>
-      <c r="B19">
-        <v>52</v>
-      </c>
-      <c r="C19">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="3">
-        <v>42044</v>
-      </c>
-      <c r="B20">
-        <v>50</v>
-      </c>
-      <c r="C20">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="3">
-        <v>42045</v>
-      </c>
-      <c r="B21">
-        <v>43</v>
-      </c>
-      <c r="C21">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="3">
-        <v>42046</v>
-      </c>
-      <c r="B22">
-        <v>31</v>
-      </c>
-      <c r="C22">
+      <c r="C39">
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="3">
-        <v>42047</v>
-      </c>
-      <c r="B23">
-        <v>22</v>
-      </c>
-      <c r="C23">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="3">
-        <v>42048</v>
-      </c>
-      <c r="C24">
+    <row r="40" spans="1:3">
+      <c r="A40" s="3">
+        <v>42055</v>
+      </c>
+      <c r="B40">
+        <v>25</v>
+      </c>
+      <c r="C40">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="3">
+        <v>42056</v>
+      </c>
+      <c r="B41">
+        <v>18</v>
+      </c>
+      <c r="C41">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="3">
+        <v>42057</v>
+      </c>
+      <c r="B42">
+        <v>14</v>
+      </c>
+      <c r="C42">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="3">
-        <v>42049</v>
-      </c>
-      <c r="C25">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="3">
-        <v>42050</v>
-      </c>
-      <c r="C26">
+    <row r="43" spans="1:3">
+      <c r="A43" s="3">
+        <v>42058</v>
+      </c>
+      <c r="B43">
+        <v>10</v>
+      </c>
+      <c r="C43">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="3">
+        <v>42059</v>
+      </c>
+      <c r="C44">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="3">
+        <v>42060</v>
+      </c>
+      <c r="C45">
         <v>0</v>
       </c>
     </row>
@@ -3257,186 +3369,175 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:C20"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="3">
-        <v>42051</v>
+        <v>42061</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="3">
-        <v>42052</v>
+        <v>42062</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D6">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="3">
-        <v>42053</v>
+        <v>42063</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C7">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D7">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="3">
-        <v>42054</v>
+        <v>42064</v>
       </c>
       <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="B9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9">
         <v>18</v>
       </c>
-      <c r="C8">
-        <v>4</v>
-      </c>
-      <c r="D8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="3">
-        <v>42055</v>
-      </c>
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9">
-        <v>6</v>
-      </c>
       <c r="D9">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10">
-        <v>20</v>
-      </c>
-      <c r="D10">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="3"/>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="2"/>
+      <c r="A12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="2"/>
+      <c r="A13" s="3">
+        <v>42061</v>
+      </c>
+      <c r="C13">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="3">
+        <v>42062</v>
+      </c>
+      <c r="C14">
+        <v>18</v>
+      </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" t="s">
-        <v>28</v>
+      <c r="A15" s="3">
+        <v>42063</v>
+      </c>
+      <c r="C15">
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="3">
-        <v>42051</v>
+        <v>42064</v>
       </c>
       <c r="C16">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="3">
-        <v>42052</v>
-      </c>
-      <c r="C17">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="3">
-        <v>42053</v>
-      </c>
-      <c r="C18">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="3">
-        <v>42054</v>
-      </c>
-      <c r="C19">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="3">
-        <v>42055</v>
-      </c>
-      <c r="C20">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="17" spans="1:1">
+      <c r="A17" s="3"/>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="3"/>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="3"/>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="3"/>
+    </row>
+    <row r="21" spans="1:1">
       <c r="A21" s="3"/>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:1">
       <c r="A22" s="3"/>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="3"/>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3446,215 +3547,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D24"/>
-  <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="24" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="3">
-        <v>42056</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="3">
-        <v>42057</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="3">
-        <v>42058</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="3">
-        <v>42059</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8">
-        <v>4</v>
-      </c>
-      <c r="D8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="3">
-        <v>42060</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9">
-        <v>4</v>
-      </c>
-      <c r="D9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="3">
-        <v>42061</v>
-      </c>
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10">
-        <v>3</v>
-      </c>
-      <c r="D10">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="3"/>
-      <c r="B11" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11">
-        <v>16</v>
-      </c>
-      <c r="D11">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="3"/>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="3">
-        <v>42056</v>
-      </c>
-      <c r="C17">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="3">
-        <v>42057</v>
-      </c>
-      <c r="C18">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="3">
-        <v>42058</v>
-      </c>
-      <c r="C19">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="3">
-        <v>42059</v>
-      </c>
-      <c r="C20">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="3">
-        <v>42060</v>
-      </c>
-      <c r="C21">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="3">
-        <v>42061</v>
-      </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="3"/>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:C19"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3667,163 +3563,150 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="3">
-        <v>42062</v>
+        <v>42065</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="3">
-        <v>42063</v>
+        <v>42066</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D6">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="3">
-        <v>42064</v>
+        <v>42067</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D7">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="3">
-        <v>42065</v>
+        <v>42068</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D8">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="3">
-        <v>42066</v>
-      </c>
-      <c r="B9" t="s">
-        <v>21</v>
+      <c r="A9" s="3"/>
+      <c r="B9" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="C9">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="D9">
-        <v>6</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="3"/>
-      <c r="B10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10">
-        <v>17</v>
-      </c>
-      <c r="D10">
-        <v>34</v>
-      </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2"/>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="2"/>
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="3">
+        <v>42065</v>
+      </c>
+      <c r="C13">
+        <v>36</v>
+      </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" t="s">
-        <v>28</v>
+      <c r="A14" s="3">
+        <v>42066</v>
+      </c>
+      <c r="C14">
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="3">
-        <v>42062</v>
+        <v>42067</v>
       </c>
       <c r="C15">
-        <v>32</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="3">
-        <v>42063</v>
+        <v>42068</v>
       </c>
       <c r="C16">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="3">
-        <v>42064</v>
-      </c>
-      <c r="C17">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="3">
-        <v>42065</v>
-      </c>
-      <c r="C18">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="3">
-        <v>42066</v>
-      </c>
-      <c r="C19">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="17" spans="1:1">
+      <c r="A17" s="3"/>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="3"/>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="3"/>
+    </row>
+    <row r="20" spans="1:1">
       <c r="A20" s="3"/>
     </row>
   </sheetData>
@@ -3832,178 +3715,167 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.85546875" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" customWidth="1"/>
     <col min="3" max="3" width="19.140625" customWidth="1"/>
     <col min="4" max="4" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="3">
-        <v>42067</v>
+        <v>42069</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D5">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="3">
-        <v>42068</v>
+        <v>42070</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D6">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="3">
-        <v>42069</v>
+        <v>42071</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D7">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="3">
-        <v>42070</v>
+        <v>42072</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="B9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="3">
-        <v>42071</v>
-      </c>
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
       <c r="C9">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="D9">
-        <v>6</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="3"/>
-      <c r="B10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10">
-        <v>16</v>
-      </c>
-      <c r="D10">
-        <v>32</v>
-      </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2"/>
     </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="3">
+        <v>42069</v>
+      </c>
+      <c r="C13">
+        <v>32</v>
+      </c>
+    </row>
     <row r="14" spans="1:4">
-      <c r="A14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" t="s">
-        <v>28</v>
+      <c r="A14" s="3">
+        <v>42070</v>
+      </c>
+      <c r="C14">
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="3">
-        <v>42067</v>
+        <v>42071</v>
       </c>
       <c r="C15">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="3">
-        <v>42068</v>
+        <v>42072</v>
       </c>
       <c r="C16">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="3">
-        <v>42069</v>
-      </c>
-      <c r="C17">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="3">
-        <v>42070</v>
-      </c>
-      <c r="C18">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="3">
-        <v>42071</v>
-      </c>
-      <c r="C19">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="17" spans="1:1">
+      <c r="A17" s="3"/>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="3"/>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="3"/>
+    </row>
+    <row r="20" spans="1:1">
       <c r="A20" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added menus stage 4 to stage 9
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="15315" windowHeight="5955" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="15315" windowHeight="5955" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="37">
   <si>
     <t>Product Backlog</t>
   </si>
@@ -410,24 +410,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="57513088"/>
-        <c:axId val="57514624"/>
+        <c:axId val="65967232"/>
+        <c:axId val="65968768"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="57513088"/>
+        <c:axId val="65967232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="[$-409]mmmm\ d\,\ yyyy;@" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57514624"/>
+        <c:crossAx val="65968768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="57514624"/>
+        <c:axId val="65968768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -435,7 +435,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57513088"/>
+        <c:crossAx val="65967232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -461,7 +461,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -725,24 +725,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="57805056"/>
-        <c:axId val="57827328"/>
+        <c:axId val="67307776"/>
+        <c:axId val="67330048"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="57805056"/>
+        <c:axId val="67307776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="[$-409]mmmm\ d\,\ yyyy;@" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57827328"/>
+        <c:crossAx val="67330048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="57827328"/>
+        <c:axId val="67330048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -750,7 +750,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57805056"/>
+        <c:crossAx val="67307776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -762,7 +762,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1053,24 +1053,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="57893632"/>
-        <c:axId val="57895168"/>
+        <c:axId val="67392256"/>
+        <c:axId val="67393792"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="57893632"/>
+        <c:axId val="67392256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="[$-409]mmmm\ d\,\ yyyy;@" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57895168"/>
+        <c:crossAx val="67393792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="57895168"/>
+        <c:axId val="67393792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1078,7 +1078,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57893632"/>
+        <c:crossAx val="67392256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1090,7 +1090,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1163,6 +1163,9 @@
                 <c:pt idx="3">
                   <c:v>5</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1234,24 +1237,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="58989184"/>
-        <c:axId val="58999168"/>
+        <c:axId val="67443328"/>
+        <c:axId val="67453312"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="58989184"/>
+        <c:axId val="67443328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="[$-409]mmmm\ d\,\ yyyy;@" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58999168"/>
+        <c:crossAx val="67453312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="58999168"/>
+        <c:axId val="67453312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1259,20 +1262,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58989184"/>
+        <c:crossAx val="67443328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1330,6 +1332,15 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1395,24 +1406,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="68370816"/>
-        <c:axId val="68372352"/>
+        <c:axId val="67584384"/>
+        <c:axId val="67585920"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="68370816"/>
+        <c:axId val="67584384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="[$-409]mmmm\ d\,\ yyyy;@" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68372352"/>
+        <c:crossAx val="67585920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="68372352"/>
+        <c:axId val="67585920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1420,7 +1431,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68370816"/>
+        <c:crossAx val="67584384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1432,7 +1443,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1465,17 +1476,23 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sprint 6'!$A$13:$A$16</c:f>
+              <c:f>'Sprint 6'!$A$13:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>[$-409]mmmm\ d\,\ yyyy;@</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
+                  <c:v>42068</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42069</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>42070</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>42071</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>42072</c:v>
                 </c:pt>
               </c:numCache>
@@ -1483,10 +1500,25 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 6'!$B$13:$B$16</c:f>
+              <c:f>'Sprint 6'!$B$13:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1510,17 +1542,23 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sprint 6'!$A$13:$A$16</c:f>
+              <c:f>'Sprint 6'!$A$13:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>[$-409]mmmm\ d\,\ yyyy;@</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
+                  <c:v>42068</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42069</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>42070</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>42071</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>42072</c:v>
                 </c:pt>
               </c:numCache>
@@ -1528,17 +1566,23 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 6'!$C$13:$C$16</c:f>
+              <c:f>'Sprint 6'!$C$13:$C$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1546,24 +1590,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="68405504"/>
-        <c:axId val="68411392"/>
+        <c:axId val="67619072"/>
+        <c:axId val="67624960"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="68405504"/>
+        <c:axId val="67619072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="[$-409]mmmm\ d\,\ yyyy;@" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68411392"/>
+        <c:crossAx val="67624960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="68411392"/>
+        <c:axId val="67624960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1571,19 +1615,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68405504"/>
+        <c:crossAx val="67619072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1769,19 +1814,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2847,7 +2892,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
@@ -3390,8 +3435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3564,6 +3609,9 @@
       <c r="A17" s="3">
         <v>42065</v>
       </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
       <c r="C17">
         <v>0</v>
       </c>
@@ -3599,8 +3647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3719,6 +3767,9 @@
       <c r="A13" s="3">
         <v>42066</v>
       </c>
+      <c r="B13">
+        <v>34</v>
+      </c>
       <c r="C13">
         <v>36</v>
       </c>
@@ -3727,6 +3778,9 @@
       <c r="A14" s="3">
         <v>42067</v>
       </c>
+      <c r="B14">
+        <v>20</v>
+      </c>
       <c r="C14">
         <v>24</v>
       </c>
@@ -3734,6 +3788,9 @@
     <row r="15" spans="1:4">
       <c r="A15" s="3">
         <v>42068</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
       </c>
       <c r="C15">
         <v>12</v>
@@ -3769,8 +3826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3802,7 +3859,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="3">
-        <v>42070</v>
+        <v>42068</v>
       </c>
       <c r="B5" t="s">
         <v>28</v>
@@ -3816,46 +3873,71 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="3">
-        <v>42071</v>
+        <v>42069</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="C6">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D6">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="3">
+        <v>42070</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="3">
+        <v>42071</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="3">
         <v>42072</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B9" t="s">
         <v>16</v>
       </c>
-      <c r="C7">
-        <v>10</v>
-      </c>
-      <c r="D7">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4" t="s">
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
         <v>4</v>
-      </c>
-      <c r="C8">
-        <v>20</v>
-      </c>
-      <c r="D8">
-        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="3"/>
+      <c r="B10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>20</v>
+      </c>
+      <c r="D10">
+        <v>40</v>
+      </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2"/>
@@ -3873,7 +3955,10 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="3">
-        <v>42070</v>
+        <v>42068</v>
+      </c>
+      <c r="B13">
+        <v>20</v>
       </c>
       <c r="C13">
         <v>32</v>
@@ -3881,33 +3966,55 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="3">
-        <v>42071</v>
+        <v>42069</v>
+      </c>
+      <c r="B14">
+        <v>15</v>
       </c>
       <c r="C14">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="3">
+        <v>42070</v>
+      </c>
+      <c r="B15">
+        <v>10</v>
+      </c>
+      <c r="C15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="3">
+        <v>42071</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="3">
         <v>42072</v>
       </c>
-      <c r="C15">
+      <c r="B17">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="3"/>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="3"/>
-    </row>
-    <row r="18" spans="1:1">
+      <c r="C17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="3"/>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:3">
       <c r="A19" s="3"/>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:3">
       <c r="A20" s="3"/>
     </row>
   </sheetData>

</xml_diff>